<commit_message>
bug fix and structurally improved bar chart
used faceting to separate months, and normalised all OTU abundances to relative percentages
</commit_message>
<xml_diff>
--- a/outputs/tables/distest_medianmetal.xlsx
+++ b/outputs/tables/distest_medianmetal.xlsx
@@ -1,117 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarprice/Documents/University/Year 3/Term 1/Dissertation/R/Dissertation/outputs/tables/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1F5057-0AA3-2E4C-9FF0-2F62B6BC44D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="0" windowWidth="16800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Metal</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>p.value</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Aluminium_median.μgL</t>
-  </si>
-  <si>
-    <t>Arsenic_median.μgL</t>
-  </si>
-  <si>
-    <t>Barium_median.μgL</t>
-  </si>
-  <si>
-    <t>Boron_median.μgL</t>
-  </si>
-  <si>
-    <t>Constant values</t>
-  </si>
-  <si>
-    <t>Cadmium_median.μgL</t>
-  </si>
-  <si>
-    <t>Calcium_median.μgL</t>
-  </si>
-  <si>
-    <t>Chromium_median.μgL</t>
-  </si>
-  <si>
-    <t>Copper_median.μgL</t>
-  </si>
-  <si>
-    <t>Iron_median.μgL</t>
-  </si>
-  <si>
-    <t>Lead_median.μgL</t>
-  </si>
-  <si>
-    <t>Lithium_median.μgL</t>
-  </si>
-  <si>
-    <t>Magnesium_median.μgL</t>
-  </si>
-  <si>
-    <t>Manganese_median.μgL</t>
-  </si>
-  <si>
-    <t>Nickel_median.μgL</t>
-  </si>
-  <si>
-    <t>Potassium_median.μgL</t>
-  </si>
-  <si>
-    <t>Sodium_median.μgL</t>
-  </si>
-  <si>
-    <t>Zinc_median.μgL</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,34 +52,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +107,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -247,7 +141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -282,10 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,263 +350,305 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.52841156274445011</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3.6784123725175361E-6</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metal</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p.value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Aluminium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>0.5284115627444501</v>
+      </c>
+      <c r="C2">
+        <v>3.678412372517536E-06</v>
       </c>
       <c r="D2">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.77491615653331458</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.289051735839615E-3</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Arsenic_median.μgL</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.7749161565333146</v>
+      </c>
+      <c r="C3">
+        <v>0.001289051735839615</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.71147845490715977</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2.26430912531105E-4</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Barium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>0.7114784549071598</v>
+      </c>
+      <c r="C4">
+        <v>0.000226430912531105</v>
       </c>
       <c r="D4">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Boron_median.μgL</t>
+        </is>
+      </c>
       <c r="D5">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.80403406004542677</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3.0825794528095678E-3</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Constant values</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cadmium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.8040340600454268</v>
+      </c>
+      <c r="C6">
+        <v>0.003082579452809568</v>
       </c>
       <c r="D6">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.79451205048405726</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2.30491441908932E-3</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Calcium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>0.7945120504840573</v>
+      </c>
+      <c r="C7">
+        <v>0.00230491441908932</v>
       </c>
       <c r="D7">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Chromium_median.μgL</t>
+        </is>
+      </c>
       <c r="D8">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.81616156993912203</v>
-      </c>
-      <c r="C9" s="3">
-        <v>4.5009928902073606E-3</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Constant values</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Copper_median.μgL</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>0.816161569939122</v>
+      </c>
+      <c r="C9">
+        <v>0.004500992890207361</v>
       </c>
       <c r="D9">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.70914790715391429</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2.1320759412365639E-4</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Iron_median.μgL</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>0.7091479071539143</v>
+      </c>
+      <c r="C10">
+        <v>0.0002132075941236564</v>
       </c>
       <c r="D10">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.67509757958819672</v>
-      </c>
-      <c r="C11" s="3">
-        <v>9.0894260169089723E-5</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lead_median.μgL</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0.6750975795881967</v>
+      </c>
+      <c r="C11">
+        <v>9.089426016908972E-05</v>
       </c>
       <c r="D11">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.27265492268640917</v>
-      </c>
-      <c r="C12" s="3">
-        <v>4.5531081654202947E-8</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lithium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>0.2726549226864092</v>
+      </c>
+      <c r="C12">
+        <v>4.553108165420295E-08</v>
       </c>
       <c r="D12">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.81538589885514468</v>
-      </c>
-      <c r="C13" s="3">
-        <v>4.3920869223267756E-3</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Magnesium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>0.8153858988551447</v>
+      </c>
+      <c r="C13">
+        <v>0.004392086922326776</v>
       </c>
       <c r="D13">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.70498893160260101</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.9161421332520291E-4</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Manganese_median.μgL</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>0.704988931602601</v>
+      </c>
+      <c r="C14">
+        <v>0.0001916142133252029</v>
       </c>
       <c r="D14">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.70301243219841314</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1.8218162892125379E-4</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nickel_median.μgL</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>0.7030124321984131</v>
+      </c>
+      <c r="C15">
+        <v>0.0001821816289212538</v>
       </c>
       <c r="D15">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.95135492978737879</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.51145304195993269</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Potassium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>0.9513549297873788</v>
+      </c>
+      <c r="C16">
+        <v>0.5114530419599327</v>
       </c>
       <c r="D16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.83319980854835074</v>
-      </c>
-      <c r="C17" s="3">
-        <v>7.7859460832327343E-3</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Sodium_median.μgL</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>0.8331998085483507</v>
+      </c>
+      <c r="C17">
+        <v>0.007785946083232734</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.80680108691808927</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3.357873727998601E-3</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Zinc_median.μgL</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>0.8068010869180893</v>
+      </c>
+      <c r="C18">
+        <v>0.003357873727998601</v>
       </c>
       <c r="D18">
         <v>16</v>

</xml_diff>